<commit_message>
Diagram OK + bug fix.
</commit_message>
<xml_diff>
--- a/asset/diagram.xlsx
+++ b/asset/diagram.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/TP_Villes_du_Monde/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D00F15B-8DBD-2C43-9009-1F0A7049B276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732F2CD3-E1CB-794E-B965-F3E919781795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{8735055C-E134-3E4D-82DA-80B73531BE17}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{8735055C-E134-3E4D-82DA-80B73531BE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="Param" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Diagram!$C$1:$M$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Diagram!$A$1:$R$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
   <si>
     <t>dataSource</t>
   </si>
@@ -62,9 +62,6 @@
     <t>class AbstractButton(buttonDiv)</t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
     <t>UIView</t>
   </si>
   <si>
@@ -222,6 +219,126 @@
   </si>
   <si>
     <t>Méthode d'initialisation du composant Indexer.</t>
+  </si>
+  <si>
+    <t>class SearchInput(UIView) inherit AbstractUIComponent</t>
+  </si>
+  <si>
+    <t>boundSearchInputHandler</t>
+  </si>
+  <si>
+    <t>boundClearSearchHandler</t>
+  </si>
+  <si>
+    <t>propriété pour le binding de searchInputHandler lors de la saisie de texte (voir exemple dans TP Jeu de Paires).</t>
+  </si>
+  <si>
+    <t>propriété pour le binding de clearSearchHandler lors de l'effacement de texte (voir exemple dans TP Jeu de Paires).</t>
+  </si>
+  <si>
+    <t>getter du composant (surcharge)</t>
+  </si>
+  <si>
+    <t>setter du composant (surcharge)</t>
+  </si>
+  <si>
+    <t>Méthode d'initialisation du composant (surcharge)</t>
+  </si>
+  <si>
+    <t>clearSearchHandler()</t>
+  </si>
+  <si>
+    <t>Gestionnaire exécuté lors de la saisie de texte. Dispatch un SearchInputEvent de type SearchInputEventNames.SEARCH_INPUT écouté dans l'app.</t>
+  </si>
+  <si>
+    <t>Gestionnaire exécuté lors de l'effacement du champs de texte quand on clique sur le boutton d'effacement. Dispatch un SearchInputEvent de type SearchInputEventNames.CLEAR_SEARCH_INPUT écouté dans l'app.</t>
+  </si>
+  <si>
+    <t>checkClearButton()</t>
+  </si>
+  <si>
+    <t>Désactive ou active le boutton si le champs de texte est vide ou pas.</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>class Indexer(UIView) inherit AbstractUIComponent</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>le total d'éléments.</t>
+  </si>
+  <si>
+    <t>indexerMode</t>
+  </si>
+  <si>
+    <t>Le mode (répétition, aucun, etc...)</t>
+  </si>
+  <si>
+    <t>nextBtn</t>
+  </si>
+  <si>
+    <t>Le boutton suivant</t>
+  </si>
+  <si>
+    <t>previousBtn</t>
+  </si>
+  <si>
+    <t>Le boutton précédent</t>
+  </si>
+  <si>
+    <t>setter pour définir le mode si besoin après initialisation.</t>
+  </si>
+  <si>
+    <t>set mode</t>
+  </si>
+  <si>
+    <t>set totalItems</t>
+  </si>
+  <si>
+    <t>setter pour définir le total d'éléments. Définit lors du filtrage et la réinitialisation du filtrage.</t>
+  </si>
+  <si>
+    <t>surcharge pour retourner la valeur du composant.</t>
+  </si>
+  <si>
+    <t>changeIndex(direction)</t>
+  </si>
+  <si>
+    <t>Change l'index en fonction de la direction déterminée par le clic sur les boutons suivant / précédent.</t>
+  </si>
+  <si>
+    <t>checkIndex()</t>
+  </si>
+  <si>
+    <t>Vérifie l'index en fonction du mode et le remet à 0 si out of range (voir TP Citations).</t>
+  </si>
+  <si>
+    <t>setNumbers()</t>
+  </si>
+  <si>
+    <t>getZeroFormat(num, limit)</t>
+  </si>
+  <si>
+    <t>Affiche 2/8, 06/12, etc… à l'aide de la méthode getZeroFormat().</t>
+  </si>
+  <si>
+    <t>Retourne l'index / total formaté (voir TP Citations).</t>
+  </si>
+  <si>
+    <t>initButtons()</t>
+  </si>
+  <si>
+    <t>Initialise les boutons suivant / précédent.</t>
+  </si>
+  <si>
+    <t>class IndexerButton(buttonDiv) inherit AbstractButton</t>
+  </si>
+  <si>
+    <t>Surcharge la méthode et définit une classe CSS en plus de la méthode de base.</t>
   </si>
 </sst>
 </file>
@@ -259,7 +376,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -421,6 +538,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -479,11 +616,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -497,17 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -525,28 +674,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,10 +915,10 @@
       <xdr:rowOff>195384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1133231</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>117231</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -700,8 +933,114 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13335024" y="1914769"/>
-          <a:ext cx="29284" cy="2540000"/>
+          <a:off x="14159547" y="1973384"/>
+          <a:ext cx="3722053" cy="2649416"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3235521</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>50236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connecteur droit avec flèche 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F904518E-68B7-4E49-952B-9C2424FDAB4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6649281" y="2437836"/>
+          <a:ext cx="4008559" cy="1859844"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>511280</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>110717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>237067</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connecteur droit avec flèche 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEBC8B3F-9512-3249-9F6A-A5D1ABE35161}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23354347" y="2532184"/>
+          <a:ext cx="5279920" cy="1836616"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1030,44 +1369,47 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:O38"/>
+  <dimension ref="A2:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="59" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.1640625" customWidth="1"/>
     <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="G3" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
-      <c r="K3" s="20" t="s">
+      <c r="B3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="G3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="K3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="22"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
@@ -1080,7 +1422,7 @@
       </c>
       <c r="D4" s="7" t="str">
         <f>Param!A3</f>
-        <v>Check</v>
+        <v>Checked</v>
       </c>
       <c r="G4" s="6" t="str">
         <f>Param!A1</f>
@@ -1092,7 +1434,7 @@
       </c>
       <c r="I4" s="6" t="str">
         <f>Param!A3</f>
-        <v>Check</v>
+        <v>Checked</v>
       </c>
       <c r="K4" s="6" t="str">
         <f>Param!A1</f>
@@ -1104,112 +1446,112 @@
       </c>
       <c r="M4" s="7" t="str">
         <f>Param!A3</f>
-        <v>Check</v>
+        <v>Checked</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="14"/>
+      <c r="G5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="K5" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="2:15" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="G5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="14" t="s">
+      <c r="C6" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="G6" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="K6" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="G7" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="K5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="2:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="30"/>
-      <c r="G6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="K6" s="4" t="s">
+      <c r="I7" s="5"/>
+      <c r="K7" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="33" t="s">
+      <c r="L7" s="48"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="G7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="18"/>
+      <c r="L8" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="2:15" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="K9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="17" t="s">
+      <c r="K9" s="32" t="s">
         <v>23</v>
+      </c>
+      <c r="L9" s="46" t="s">
+        <v>22</v>
       </c>
       <c r="M9" s="3"/>
     </row>
@@ -1255,9 +1597,9 @@
       <c r="F14" s="10"/>
       <c r="G14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
     </row>
@@ -1289,7 +1631,7 @@
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1303,7 +1645,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1317,7 +1659,7 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1331,12 +1673,17 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
+    <row r="20" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="E20" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -1344,209 +1691,390 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
+    <row r="21" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="str">
+        <f>Param!A1</f>
+        <v>Properties / Methods</v>
+      </c>
+      <c r="B21" s="6" t="str">
+        <f>Param!A2</f>
+        <v>Description</v>
+      </c>
+      <c r="C21" s="7" t="str">
+        <f>Param!A3</f>
+        <v>Checked</v>
+      </c>
+      <c r="E21" s="6" t="str">
+        <f>Param!A1</f>
+        <v>Properties / Methods</v>
+      </c>
+      <c r="F21" s="6" t="str">
+        <f>Param!A2</f>
+        <v>Description</v>
+      </c>
+      <c r="G21" s="6" t="str">
+        <f>Param!A3</f>
+        <v>Checked</v>
+      </c>
       <c r="J21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="9"/>
+      <c r="O21" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="18"/>
+    </row>
+    <row r="22" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="E22" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="I22" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="59"/>
+      <c r="K22" s="60"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-    </row>
-    <row r="23" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="6" t="str">
+      <c r="O22" s="6" t="str">
         <f>Param!A1</f>
         <v>Properties / Methods</v>
       </c>
-      <c r="H23" s="36" t="str">
+      <c r="P22" s="7" t="str">
         <f>Param!A2</f>
         <v>Description</v>
       </c>
+      <c r="Q22" s="7" t="str">
+        <f>Param!A3</f>
+        <v>Checked</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="E23" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="4"/>
       <c r="I23" s="6" t="str">
+        <f>Param!A1</f>
+        <v>Properties / Methods</v>
+      </c>
+      <c r="J23" s="26" t="str">
+        <f>Param!A2</f>
+        <v>Description</v>
+      </c>
+      <c r="K23" s="6" t="str">
         <f>Param!A3</f>
-        <v>Check</v>
-      </c>
-      <c r="J23" s="9"/>
+        <v>Checked</v>
+      </c>
       <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="2:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="14" t="s">
+      <c r="O23" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="P23" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="E24" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="I24" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="9"/>
+      <c r="K24" s="13"/>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
-    </row>
-    <row r="25" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="G25" s="4" t="s">
+      <c r="P24" s="20"/>
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="E25" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="I25" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="9"/>
+      <c r="K25" s="4"/>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
-    </row>
-    <row r="26" spans="2:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="G26" s="4" t="s">
+      <c r="P25" s="20"/>
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="E26" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="I26" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="K26" s="4"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="9"/>
+    </row>
+    <row r="27" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A27" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="E27" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="I27" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="2:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="G27" s="29" t="s">
+      <c r="J27" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="K27" s="4"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="9"/>
+    </row>
+    <row r="28" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+      <c r="A28" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="E28" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="I28" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="2:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="G28" s="28" t="s">
+      <c r="J28" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="K28" s="25"/>
+    </row>
+    <row r="29" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="E29" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="I29" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="35"/>
-    </row>
-    <row r="29" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="G29" s="29" t="s">
+      <c r="J29" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="H29" s="25" t="s">
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="E30" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="I30" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="2:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="G30" s="29" t="s">
+      <c r="J30" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="H30" s="25" t="s">
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="E31" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="I31" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="2:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="G31" s="29" t="s">
+      <c r="J31" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="H31" s="25" t="s">
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="E32" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="I32" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="2:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="G32" s="29" t="s">
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="5:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="E33" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="I33" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="H32" s="25" t="s">
+      <c r="J33" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="7:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="G33" s="29" t="s">
+      <c r="K33" s="4"/>
+    </row>
+    <row r="34" spans="5:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="I34" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="7:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="G34" s="29" t="s">
+      <c r="J34" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="5:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="I35" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="7:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="G35" s="29" t="s">
+      <c r="J35" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="25" t="s">
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="5:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="I36" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="7:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="G36" s="29" t="s">
+      <c r="J36" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="5:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="I37" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="7:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="G37" s="29" t="s">
+      <c r="J37" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="H37" s="25" t="s">
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="5:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="7:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G38" s="15" t="s">
+      <c r="J38" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="H38" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38" s="5"/>
+      <c r="K38" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="O21:Q21"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="E20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="51" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="29" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1576,7 +2104,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>